<commit_message>
Calcular IGV en OC
</commit_message>
<xml_diff>
--- a/bk/PROCEDURES_FEROZO.xlsx
+++ b/bk/PROCEDURES_FEROZO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseHernan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\constructora\bk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D62DE06-D0E2-4997-BC3D-807A394A7AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413142FF-8B99-4A6B-AEF6-61F039AAA892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3D021364-6B44-41FE-AFA0-9D1DE1DF3836}"/>
   </bookViews>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -164,10 +158,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,9 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D095DF-38D2-4FAE-B920-03E0B2D138D1}">
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -497,7 +490,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="str">

</xml_diff>